<commit_message>
Added birthdays and changed email id
</commit_message>
<xml_diff>
--- a/data/Birthdays.xlsx
+++ b/data/Birthdays.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swetha\JenkinsPipeline\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swaminsw\BirthdayProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAE695D-AC0E-4569-8940-570B7144C674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8650F9-62F5-410F-9138-252F45394A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -58,9 +58,6 @@
     <t>17/03</t>
   </si>
   <si>
-    <t>Hona</t>
-  </si>
-  <si>
     <t>Ashrith</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>03/03</t>
   </si>
   <si>
-    <t>05/10</t>
-  </si>
-  <si>
     <t>16/08</t>
   </si>
   <si>
@@ -146,13 +140,37 @@
   </si>
   <si>
     <t>06/05</t>
+  </si>
+  <si>
+    <t>21/06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mythili </t>
+  </si>
+  <si>
+    <t>Jugil</t>
+  </si>
+  <si>
+    <t>26/06</t>
+  </si>
+  <si>
+    <t>Sawan</t>
+  </si>
+  <si>
+    <t>Deepali</t>
+  </si>
+  <si>
+    <t>11/02</t>
+  </si>
+  <si>
+    <t>04/08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -172,6 +190,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,7 +204,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,22 +212,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +462,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -447,31 +486,31 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
+      <c r="B2" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>25</v>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -479,146 +518,163 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>26</v>
+      <c r="B6" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>30</v>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
+      <c r="A11" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>32</v>
+      <c r="A12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>35</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>36</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="5"/>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added udaan and vimaan
</commit_message>
<xml_diff>
--- a/data/Birthdays.xlsx
+++ b/data/Birthdays.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swaminsw\BirthdayProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8650F9-62F5-410F-9138-252F45394A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718D56D6-E76A-4AD5-A2FC-5B3BA0336537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Sushrutha</t>
   </si>
   <si>
-    <t>Sreeja</t>
-  </si>
-  <si>
     <t>Kratika</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>26/09</t>
   </si>
   <si>
-    <t>16/02</t>
-  </si>
-  <si>
     <t>15/11</t>
   </si>
   <si>
@@ -164,6 +158,117 @@
   </si>
   <si>
     <t>04/08</t>
+  </si>
+  <si>
+    <t>Chandra</t>
+  </si>
+  <si>
+    <t>21/09</t>
+  </si>
+  <si>
+    <t>Pradeep</t>
+  </si>
+  <si>
+    <t>20/09</t>
+  </si>
+  <si>
+    <t>Sumi</t>
+  </si>
+  <si>
+    <t>Vaibhav</t>
+  </si>
+  <si>
+    <t>20/03</t>
+  </si>
+  <si>
+    <t>Koti</t>
+  </si>
+  <si>
+    <t>30/12</t>
+  </si>
+  <si>
+    <t>Nithish</t>
+  </si>
+  <si>
+    <t>09/10</t>
+  </si>
+  <si>
+    <t>Suhas</t>
+  </si>
+  <si>
+    <t>19/12</t>
+  </si>
+  <si>
+    <t>17/08</t>
+  </si>
+  <si>
+    <t>14/08</t>
+  </si>
+  <si>
+    <t>Aronya</t>
+  </si>
+  <si>
+    <t>10/10</t>
+  </si>
+  <si>
+    <t>22/04</t>
+  </si>
+  <si>
+    <t>14/10</t>
+  </si>
+  <si>
+    <t>28/04</t>
+  </si>
+  <si>
+    <t>03/12</t>
+  </si>
+  <si>
+    <t>14/03</t>
+  </si>
+  <si>
+    <t>13/11</t>
+  </si>
+  <si>
+    <t>03/04</t>
+  </si>
+  <si>
+    <t>25/10</t>
+  </si>
+  <si>
+    <t>Avijit</t>
+  </si>
+  <si>
+    <t>Vinod</t>
+  </si>
+  <si>
+    <t>Kalpana</t>
+  </si>
+  <si>
+    <t>Eslyn</t>
+  </si>
+  <si>
+    <t>Vijayashree</t>
+  </si>
+  <si>
+    <t>Reshma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinay </t>
+  </si>
+  <si>
+    <t>Priyanka</t>
+  </si>
+  <si>
+    <t>Khushal</t>
+  </si>
+  <si>
+    <t>Prem</t>
+  </si>
+  <si>
+    <t>Biplab</t>
+  </si>
+  <si>
+    <t>Pritish</t>
   </si>
 </sst>
 </file>
@@ -231,18 +336,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,10 +569,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -478,7 +585,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -486,31 +593,31 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>24</v>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -518,160 +625,392 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>25</v>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>46</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>43</v>
+      <c r="A11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>40</v>
+      <c r="A12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>